<commit_message>
Cleaned up names and moved irrelevant shit into misc folder
</commit_message>
<xml_diff>
--- a/Hubble.xlsx
+++ b/Hubble.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TheBestKid/Desktop/Hubble/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7F9B23F-8C0A-6E4A-9D71-071301B147CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D50188-8FA8-B043-B38F-08636DDE0EC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="3060" windowWidth="26840" windowHeight="15940" xr2:uid="{E5F18B58-E478-4F41-B9E4-06DCA8F0E8B0}"/>
+    <workbookView xWindow="1120" yWindow="820" windowWidth="26840" windowHeight="15940" xr2:uid="{E5F18B58-E478-4F41-B9E4-06DCA8F0E8B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hubble" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -230,7 +230,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$6</c:f>
+              <c:f>Hubble!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -254,21 +254,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$6</c:f>
+              <c:f>Hubble!$H$2:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>432513831.03500867</c:v>
+                  <c:v>432.51383103500865</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>588843655.35558987</c:v>
+                  <c:v>588.84365535558982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>797994687.26798081</c:v>
+                  <c:v>797.99468726798079</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1294195841.4499903</c:v>
+                  <c:v>1294.1958414499902</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,8 +1424,8 @@
         <v>0.105</v>
       </c>
       <c r="H2">
-        <f>10^((D2+22.1 +5)/5)</f>
-        <v>432513831.03500867</v>
+        <f>(10^((D2+22.1 +5)/5))/(10^6)</f>
+        <v>432.51383103500865</v>
       </c>
       <c r="I2">
         <f>G2*(3*10^5)</f>
@@ -1455,8 +1455,8 @@
         <v>0.152</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H5" si="0">10^((D3+22.1 +5)/5)</f>
-        <v>588843655.35558987</v>
+        <f t="shared" ref="H3:H5" si="0">(10^((D3+22.1 +5)/5))/(10^6)</f>
+        <v>588.84365535558982</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I5" si="1">G3*(3*10^5)</f>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>797994687.26798081</v>
+        <v>797.99468726798079</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1294195841.4499903</v>
+        <v>1294.1958414499902</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
@@ -1546,6 +1546,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>